<commit_message>
Filtered out non-regular volumes like protocol endpoints, and don't tag them in staas-tag_vols.
Moved common code to staas-common

Changed USER_NAME and API_KEY variables to environment variables instead of being imported from the STAAS_Tagging spreadsheet
</commit_message>
<xml_diff>
--- a/STAAS_Tagging.xlsx
+++ b/STAAS_Tagging.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\prosham\Src\staas-provisioning-fusion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\prosham\Src\STAAS-Reporting-Fusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8317F64E-5D92-4B6D-97CF-33B7E7E80F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B677992-268C-4AE2-9DF9-0950DD91740F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9248" yWindow="8940" windowWidth="23864" windowHeight="14317" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1222" yWindow="11190" windowWidth="33841" windowHeight="10095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fleet" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>App1</t>
   </si>
@@ -47,15 +47,6 @@
     <t>App8</t>
   </si>
   <si>
-    <t>USER_NAME</t>
-  </si>
-  <si>
-    <t>prosham</t>
-  </si>
-  <si>
-    <t>5887696c-bceb-1ea1-77df-f316fb18c090</t>
-  </si>
-  <si>
     <t>FUSION_SERVER</t>
   </si>
   <si>
@@ -68,9 +59,6 @@
     <t>Telstra-STAAS</t>
   </si>
   <si>
-    <t>API_TOKEN</t>
-  </si>
-  <si>
     <t>Application</t>
   </si>
   <si>
@@ -144,21 +132,6 @@
   </si>
   <si>
     <t>App32</t>
-  </si>
-  <si>
-    <t>Accessed_By</t>
-  </si>
-  <si>
-    <t>Host</t>
-  </si>
-  <si>
-    <t>HostGroup</t>
-  </si>
-  <si>
-    <t>VM</t>
-  </si>
-  <si>
-    <t>Static</t>
   </si>
   <si>
     <t>IT</t>
@@ -471,229 +444,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C44270D-3563-0E45-A338-3DEA83E1D2E2}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E11" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E12" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E13" t="s">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E14" t="s">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E15" t="s">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E16" t="s">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E17" t="s">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E18" t="s">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E19" t="s">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E20" t="s">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E21" t="s">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E22" t="s">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E23" t="s">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E24" t="s">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E25" t="s">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E26" t="s">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E27" t="s">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E28" t="s">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E29" t="s">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E30" t="s">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E34" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -721,23 +664,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1">
         <v>1000</v>
@@ -747,10 +690,10 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>1001</v>
@@ -760,10 +703,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>1002</v>
@@ -773,10 +716,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>1003</v>
@@ -786,10 +729,10 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>1004</v>
@@ -799,10 +742,10 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>1005</v>

</xml_diff>